<commit_message>
#275493 Tweak for prod poor performance, add new err handling
</commit_message>
<xml_diff>
--- a/PlaywrightTests/CMB/PROD/Catalog_scf_XLSX.xlsx
+++ b/PlaywrightTests/CMB/PROD/Catalog_scf_XLSX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://proactis-my.sharepoint.com/personal/wai-ho_leung_proactis_com/Documents/Documents/eCat/Test Data/CM PROD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RegoMarketplace\smoke-auto-cm\PlaywrightTests\CMB\PROD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:4000b_{7BE5815B-3DFD-4CBE-8DA5-9F4D878EAE5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA06ED19-20A3-4195-AE28-81CCDEAA0A85}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78EF54C0-E74E-4EAC-8038-C0886E2111AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-45" windowWidth="38640" windowHeight="21240" tabRatio="606" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12750" yWindow="1275" windowWidth="20985" windowHeight="9705" tabRatio="606" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="3" r:id="rId1"/>
@@ -29,12 +29,25 @@
     <definedName name="BA_UOM" localSheetId="7">UOM!$A$5:$E$31</definedName>
     <definedName name="CODE" localSheetId="4">'Country code'!$A$5:$B$243</definedName>
   </definedNames>
-  <calcPr calcId="114210"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2062" uniqueCount="1579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2064" uniqueCount="1580">
   <si>
     <t>La description courte de l'article ne devrait pas contenir d'abréviations inconnues. De plus, le nom de l'article devrait apparaître en premier, suivi des informations d'article les plus pertinentes. Les champs de données ne doivent pas contenir de caractères de contrôle (tabulations, fin de ligne, etc.).</t>
   </si>
@@ -4893,7 +4906,10 @@
     <t>Test Image 4</t>
   </si>
   <si>
-    <t>8</t>
+    <t>TestLogo.png</t>
+  </si>
+  <si>
+    <t>TestLog2.png</t>
   </si>
 </sst>
 </file>
@@ -8453,9 +8469,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BK10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="S3" sqref="S3:S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="12.75"/>
@@ -8744,7 +8760,7 @@
         <v>1190</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="E3" s="15" t="s">
         <v>1191</v>
@@ -8772,6 +8788,9 @@
       </c>
       <c r="R3" s="15" t="s">
         <v>1198</v>
+      </c>
+      <c r="S3" s="15" t="s">
+        <v>1578</v>
       </c>
       <c r="T3" s="15" t="s">
         <v>1197</v>
@@ -8800,7 +8819,7 @@
         <v>1203</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>1196</v>
+        <v>1203</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>1191</v>
@@ -8828,6 +8847,9 @@
       </c>
       <c r="R4" s="15" t="s">
         <v>1198</v>
+      </c>
+      <c r="S4" s="15" t="s">
+        <v>1579</v>
       </c>
       <c r="T4" s="15" t="s">
         <v>1197</v>
@@ -8850,7 +8872,7 @@
         <v>1206</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>1191</v>
@@ -8903,7 +8925,7 @@
         <v>1210</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>1191</v>
@@ -8956,7 +8978,7 @@
         <v>1215</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>1191</v>
@@ -9006,7 +9028,7 @@
         <v>1485</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>1221</v>
+        <v>1485</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>1191</v>
@@ -9056,7 +9078,7 @@
         <v>1223</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>1226</v>
+        <v>1223</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>1196</v>
@@ -9103,7 +9125,7 @@
         <v>1223</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>1578</v>
+        <v>1223</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>1196</v>

</xml_diff>